<commit_message>
Rettelser på tekst og farver
</commit_message>
<xml_diff>
--- a/documents/tidsplan.xlsx
+++ b/documents/tidsplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Multimedie design\Flow 5\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Multimedie design\Flow 5\1_eksamensprojekt2018\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709B87CD-5D35-4458-A354-562CF7FEFE88}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B6DA98-1CE9-4C35-9B69-A23AE3336512}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Projektplanlægger</t>
   </si>
@@ -361,9 +361,6 @@
     <t>• 2. brugertest</t>
   </si>
   <si>
-    <t>• Beskrivelser</t>
-  </si>
-  <si>
     <t>• Sidste rettelser</t>
   </si>
   <si>
@@ -374,6 +371,21 @@
   </si>
   <si>
     <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>• Mobil Forside</t>
+  </si>
+  <si>
+    <t>• Mobil Projekter</t>
+  </si>
+  <si>
+    <t>• Mobil Erfaringer</t>
+  </si>
+  <si>
+    <t>• Mobil Kontakt</t>
+  </si>
+  <si>
+    <t>• Rapport</t>
   </si>
 </sst>
 </file>
@@ -870,6 +882,9 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -910,9 +925,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1337,8 +1349,8 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1363,44 +1375,44 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="B2" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="12">
-        <v>43439</v>
+        <v>43451</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="42"/>
+      <c r="L2" s="43"/>
       <c r="M2" s="14"/>
-      <c r="N2" s="41" t="s">
+      <c r="N2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="42"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="45" t="s">
+      <c r="Q2" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="46"/>
+      <c r="R2" s="47"/>
       <c r="S2" s="16"/>
-      <c r="T2" s="43" t="s">
+      <c r="T2" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="44"/>
+      <c r="U2" s="45"/>
       <c r="V2" s="17"/>
-      <c r="W2" s="47" t="s">
+      <c r="W2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="48"/>
+      <c r="X2" s="49"/>
       <c r="Y2" s="24"/>
       <c r="Z2" s="24"/>
       <c r="AA2" s="24"/>
@@ -1412,22 +1424,22 @@
       <c r="AO2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="9" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="40" t="s">
+      <c r="D3" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="40" t="s">
+      <c r="F3" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="36" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1461,12 +1473,12 @@
       </c>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="39"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="28">
         <v>43430</v>
       </c>
@@ -1594,11 +1606,11 @@
         <v>43430</v>
       </c>
       <c r="F5" s="5">
-        <v>9</v>
-      </c>
-      <c r="G5" s="49">
-        <f>(SUM(G6,G11,G17,G22)/4)</f>
-        <v>0.50624999999999998</v>
+        <v>22</v>
+      </c>
+      <c r="G5" s="35">
+        <f>(SUM(G6,G11,G17,G26)/4)</f>
+        <v>0.66874999999999996</v>
       </c>
       <c r="AI5"/>
     </row>
@@ -1792,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AI14"/>
     </row>
@@ -1848,18 +1860,18 @@
       <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="E17" s="5">
-        <v>0</v>
+      <c r="E17" s="26">
+        <v>43438</v>
       </c>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="G17" s="6">
-        <f>SUM(G18:G21)/4</f>
-        <v>0.47499999999999998</v>
+        <f>SUM(G18:G25)/8</f>
+        <v>1</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AI17"/>
     </row>
@@ -1892,14 +1904,16 @@
         <v>43444</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
-      </c>
-      <c r="E19" s="26"/>
+        <v>2</v>
+      </c>
+      <c r="E19" s="26">
+        <v>43440</v>
+      </c>
       <c r="F19" s="5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G19" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19"/>
     </row>
@@ -1908,19 +1922,19 @@
         <v>31</v>
       </c>
       <c r="C20" s="26">
-        <v>43447</v>
+        <v>43446</v>
       </c>
       <c r="D20" s="5">
-        <v>2</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E20" s="26">
+        <v>43440</v>
       </c>
       <c r="F20" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI20"/>
     </row>
@@ -1929,10 +1943,10 @@
         <v>32</v>
       </c>
       <c r="C21" s="26">
-        <v>43447</v>
+        <v>43446</v>
       </c>
       <c r="D21" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21" s="26">
         <v>43439</v>
@@ -1941,150 +1955,198 @@
         <v>1</v>
       </c>
       <c r="G21" s="6">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="AI21"/>
     </row>
     <row r="22" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="32" t="s">
-        <v>33</v>
+      <c r="B22" s="33" t="s">
+        <v>39</v>
       </c>
       <c r="C22" s="26">
-        <v>43451</v>
+        <v>43447</v>
       </c>
       <c r="D22" s="5">
-        <v>3</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E22" s="26">
+        <v>43445</v>
       </c>
       <c r="F22" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22" s="6">
-        <f>SUM(G23:G26)/4</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI22"/>
     </row>
     <row r="23" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="33" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C23" s="26">
-        <v>43451</v>
+        <v>43448</v>
       </c>
       <c r="D23" s="5">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E23" s="26">
+        <v>43445</v>
       </c>
       <c r="F23" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G23" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI23"/>
     </row>
     <row r="24" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="33" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C24" s="26">
-        <v>43451</v>
+        <v>43447</v>
       </c>
       <c r="D24" s="5">
-        <v>1</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="E24" s="26">
+        <v>43445</v>
       </c>
       <c r="F24" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24"/>
     </row>
     <row r="25" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="33" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C25" s="26">
-        <v>43452</v>
+        <v>43447</v>
       </c>
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="5">
-        <v>0</v>
+      <c r="E25" s="26">
+        <v>43439</v>
       </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI25"/>
     </row>
     <row r="26" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="34" t="s">
-        <v>37</v>
+      <c r="B26" s="32" t="s">
+        <v>33</v>
       </c>
       <c r="C26" s="26">
-        <v>43453</v>
+        <v>43451</v>
       </c>
       <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="E26" s="26">
+        <v>43448</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
       </c>
       <c r="G26" s="6">
+        <f>SUM(G27:G30)/4</f>
+        <v>0.125</v>
+      </c>
+      <c r="AI26"/>
+    </row>
+    <row r="27" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="26">
+        <v>43451</v>
+      </c>
+      <c r="D27" s="5">
+        <v>3</v>
+      </c>
+      <c r="E27" s="26">
+        <v>43448</v>
+      </c>
+      <c r="F27" s="5">
+        <v>4</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AI27"/>
+    </row>
+    <row r="28" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="26">
+        <v>43451</v>
+      </c>
+      <c r="D28" s="5">
+        <v>1</v>
+      </c>
+      <c r="E28" s="5">
         <v>0</v>
       </c>
-      <c r="AI26"/>
-    </row>
-    <row r="27" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="30"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="6"/>
-      <c r="AI27"/>
-    </row>
-    <row r="28" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="30"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="6"/>
+      <c r="F28" s="5">
+        <v>0</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
       <c r="AI28"/>
     </row>
     <row r="29" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="30"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="6"/>
+      <c r="B29" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="26">
+        <v>43452</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
       <c r="AI29"/>
     </row>
     <row r="30" spans="2:35" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="30"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="6"/>
+      <c r="B30" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="26">
+        <v>43453</v>
+      </c>
+      <c r="D30" s="5">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
       <c r="AI30"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retteler i default dokumenter
</commit_message>
<xml_diff>
--- a/documents/tidsplan.xlsx
+++ b/documents/tidsplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Multimedie design\Flow 5\1_eksamensprojekt2018\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B6DA98-1CE9-4C35-9B69-A23AE3336512}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695FA8D0-35F9-414E-8496-DD81FBDEB4F0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28560" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,12 @@
     <definedName name="Faktisk">(TidsrumIFaktisk*(Projektplanlægger!$E1&gt;0))*TidsrumIPlan</definedName>
     <definedName name="FaktiskUdOver">TidsrumIFaktisk*(Projektplanlægger!$E1&gt;0)</definedName>
     <definedName name="Plan">TidsrumIPlan*(Projektplanlægger!$C1&gt;0)</definedName>
+    <definedName name="Print_Titles" localSheetId="0">Projektplanlægger!$3:$4</definedName>
     <definedName name="ProcentdelFuldført">ProcentdelFuldførtUdOver*TidsrumIPlan</definedName>
     <definedName name="ProcentdelFuldførtUdOver">(Projektplanlægger!A$4=MEDIAN(Projektplanlægger!A$4,Projektplanlægger!$E1,Projektplanlægger!$E1+Projektplanlægger!$F1)*(Projektplanlægger!$E1&gt;0))*((Projektplanlægger!A$4&lt;(INT(Projektplanlægger!$E1+Projektplanlægger!$F1*Projektplanlægger!$G1)))+(Projektplanlægger!A$4=Projektplanlægger!$E1))*(Projektplanlægger!$G1&gt;0)</definedName>
     <definedName name="TidsrumIFaktisk">Projektplanlægger!A$4=MEDIAN(Projektplanlægger!A$4,Projektplanlægger!$E1,Projektplanlægger!$E1+Projektplanlægger!$F1-1)</definedName>
     <definedName name="TidsrumIPlan">Projektplanlægger!A$4=MEDIAN(Projektplanlægger!A$4,Projektplanlægger!$C1,Projektplanlægger!$C1+Projektplanlægger!$D1-1)</definedName>
     <definedName name="Titelområde..BO60">Projektplanlægger!$B$3:$B$4</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Projektplanlægger!$3:$4</definedName>
     <definedName name="valgt_tidsrum">Projektplanlægger!$H$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -885,6 +885,30 @@
     <xf numFmtId="9" fontId="5" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -902,30 +926,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1349,14 +1349,14 @@
   </sheetPr>
   <dimension ref="B1:BO30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="AL4" sqref="AL4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" style="2" customWidth="1"/>
     <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.44140625" style="3" customWidth="1"/>
     <col min="8" max="27" width="10.33203125" style="1" customWidth="1"/>
@@ -1375,44 +1375,42 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
       <c r="G2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="12">
-        <v>43451</v>
-      </c>
+      <c r="H2" s="12"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="43"/>
+      <c r="L2" s="37"/>
       <c r="M2" s="14"/>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="43"/>
+      <c r="O2" s="37"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="47"/>
+      <c r="R2" s="41"/>
       <c r="S2" s="16"/>
-      <c r="T2" s="44" t="s">
+      <c r="T2" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="U2" s="45"/>
+      <c r="U2" s="39"/>
       <c r="V2" s="17"/>
-      <c r="W2" s="48" t="s">
+      <c r="W2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="X2" s="49"/>
+      <c r="X2" s="43"/>
       <c r="Y2" s="24"/>
       <c r="Z2" s="24"/>
       <c r="AA2" s="24"/>
@@ -1424,22 +1422,22 @@
       <c r="AO2" s="23"/>
     </row>
     <row r="3" spans="2:67" s="9" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="D3" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="36" t="s">
+      <c r="G3" s="44" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1473,12 +1471,12 @@
       </c>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="40"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="H4" s="28">
         <v>43430</v>
       </c>
@@ -1606,11 +1604,11 @@
         <v>43430</v>
       </c>
       <c r="F5" s="5">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G5" s="35">
         <f>(SUM(G6,G11,G17,G26)/4)</f>
-        <v>0.66874999999999996</v>
+        <v>0.88749999999999996</v>
       </c>
       <c r="AI5"/>
     </row>
@@ -2057,11 +2055,11 @@
         <v>43448</v>
       </c>
       <c r="F26" s="5">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="G26" s="6">
         <f>SUM(G27:G30)/4</f>
-        <v>0.125</v>
+        <v>1</v>
       </c>
       <c r="AI26"/>
     </row>
@@ -2079,10 +2077,10 @@
         <v>43448</v>
       </c>
       <c r="F27" s="5">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G27" s="6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AI27"/>
     </row>
@@ -2096,14 +2094,14 @@
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="5">
-        <v>0</v>
+      <c r="E28" s="26">
+        <v>43451</v>
       </c>
       <c r="F28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G28" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28"/>
     </row>
@@ -2117,14 +2115,14 @@
       <c r="D29" s="5">
         <v>2</v>
       </c>
-      <c r="E29" s="5">
-        <v>0</v>
+      <c r="E29" s="26">
+        <v>43453</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI29"/>
     </row>
@@ -2138,24 +2136,19 @@
       <c r="D30" s="5">
         <v>1</v>
       </c>
-      <c r="E30" s="5">
-        <v>0</v>
+      <c r="E30" s="26">
+        <v>43454</v>
       </c>
       <c r="F30" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI30"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="N2:O2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="W2:X2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
@@ -2163,6 +2156,11 @@
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="W2:X2"/>
   </mergeCells>
   <conditionalFormatting sqref="H5:AG30">
     <cfRule type="expression" dxfId="9" priority="1">
@@ -2222,7 +2220,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.51181102362204722" bottom="0.51181102362204722" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="52" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="33" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>